<commit_message>
alterei as ordens das colunas
</commit_message>
<xml_diff>
--- a/pacientes.xlsx
+++ b/pacientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programa de Automatizacao Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE18E5D-EF15-4585-95E3-B0101F784CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6FC38C-2C21-45A4-9534-923BA24C2118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="16440" xr2:uid="{AB2A274E-4327-41E4-8C99-F2074CEF43BE}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="11835" xr2:uid="{AB2A274E-4327-41E4-8C99-F2074CEF43BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Pré-Parto</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t xml:space="preserve">FRUTAS MOLES </t>
-  </si>
-  <si>
-    <t>ARTHUR FELIPE</t>
   </si>
 </sst>
 </file>
@@ -586,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A825D7-86D7-4AD3-8FD1-97DCB320C52B}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +886,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>13</v>
       </c>
@@ -897,28 +894,25 @@
         <v>301</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="2">
         <v>302</v>
       </c>
-      <c r="C34" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="2">
         <v>303</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="2">
         <v>304</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>14</v>
       </c>
@@ -926,67 +920,67 @@
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="2">
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="2">
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="2">
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="2">
         <v>205</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="2">
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="2">
         <v>207</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="2">
         <v>208</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="2">
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="2">
         <v>210</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="2">
         <v>501</v>

</xml_diff>

<commit_message>
Atualizado para UPA e Leitos com Texto
</commit_message>
<xml_diff>
--- a/pacientes.xlsx
+++ b/pacientes.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Enfermaria" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="UTI" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="UPA" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1723,4 +1724,99 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LEITO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>NOME DO PACIENTE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>DIETA</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>OBSERVAÇÕES</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ESTAB 01</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MICHAEL</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>LIQUIDA</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ESTAB 02</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TREVOR</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>PASTOSA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ESTAB 03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>FRANKLIN</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>LIVRE</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Corrigir erro site funcionando
</commit_message>
<xml_diff>
--- a/pacientes.xlsx
+++ b/pacientes.xlsx
@@ -496,16 +496,8 @@
           <t>402</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>BARBIE</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>BRANDA</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -1611,7 +1603,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NENHUMA</t>
+          <t>ESSA OBS É UM TESTE DE PRODUÇÃO</t>
         </is>
       </c>
     </row>
@@ -1623,7 +1615,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AUGUSTO CARRARA</t>
+          <t>AUGUSTO CARRARA DE SOSUA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1631,7 +1623,11 @@
           <t>LIQUIDA</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ESSA OBS É UM TESTE DE PRODUÇÃO</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1649,7 +1645,11 @@
           <t>LIVRE</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ESSA OBS É UM TESTE DE PRODUÇÃO PODE E DEVE SER APAGADO</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">

</xml_diff>